<commit_message>
Added some changes to travel_excel.py so that it adds year/month/day to excel spreadsheet and counts total kilometers.
</commit_message>
<xml_diff>
--- a/static/files/tablica-prijevoz.xlsx
+++ b/static/files/tablica-prijevoz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\PycharmProjects\AdministrationManager\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C72A4F-EB72-42B7-84F4-46498D42C29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FC57C9-F9F4-401A-8198-7186DF82B5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="1590" windowWidth="22605" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Obrazac" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>1+2</t>
   </si>
   <si>
-    <t>DATUM PODNOŠENJA IZVJEŠĆA: ________________</t>
-  </si>
-  <si>
     <t>IZVJEŠĆE O PRIJEĐENOJ UDALJENOSTI</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Adresa stanovanja:</t>
+  </si>
+  <si>
+    <t>DATUM PODNOŠENJA IZVJEŠĆA:</t>
   </si>
 </sst>
 </file>
@@ -259,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -308,45 +308,51 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,7 +695,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="C38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,31 +707,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="A3" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -735,213 +741,213 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="21"/>
+      <c r="A5" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+        <v>17</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
+        <v>19</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="29" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
     </row>
     <row r="34" spans="1:5" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
@@ -951,73 +957,81 @@
       <c r="C34" s="3">
         <v>2</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="25"/>
+      <c r="E34" s="26"/>
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="37" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
+      <c r="A37" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A38" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="31"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
     </row>
     <row r="39" spans="1:5" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:5" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="D42" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="23"/>
+      <c r="D42" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="24"/>
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="D45" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="23"/>
+      <c r="D45" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="24"/>
     </row>
     <row r="46" spans="1:5" s="14" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D46" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="D34:E34"/>
@@ -1029,11 +1043,8 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Stored file locations in env variables (Heroku issues) - Updated xlsx files to show EUR instead of kn.
</commit_message>
<xml_diff>
--- a/static/files/tablica-prijevoz.xlsx
+++ b/static/files/tablica-prijevoz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\PycharmProjects\AdministrationManager\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\PycharmProjects\AdministrationManager\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FC57C9-F9F4-401A-8198-7186DF82B5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCBF15B-8086-4DCC-B2CE-6EF69812C1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Obrazac" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -56,9 +53,6 @@
     <t>PRI DOLASKU NA POSAO I ODLASKU S POSLA</t>
   </si>
   <si>
-    <t>Odobreni iznos za isplatu _______________ kn</t>
-  </si>
-  <si>
     <t>Na ime naknade troška prijevoza potražujem:</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>(za Školu odobrava)</t>
   </si>
   <si>
-    <t>kn (stavak 6. ili st.8. čl. 67.)</t>
-  </si>
-  <si>
     <t>Za točnost i istinitost podataka iz ovog izvješća zaposlenik jamči potpisom pod punom krivičnom i materijalnom odgovornošću.</t>
   </si>
   <si>
@@ -96,6 +87,12 @@
   </si>
   <si>
     <t>DATUM PODNOŠENJA IZVJEŠĆA:</t>
+  </si>
+  <si>
+    <t>EUR (stavak 6. ili st.8. čl. 67.)</t>
+  </si>
+  <si>
+    <t>Odobreni iznos za isplatu _______________ EUR</t>
   </si>
 </sst>
 </file>
@@ -342,17 +339,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,26 +704,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -741,16 +738,16 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>18</v>
+      <c r="A5" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
@@ -758,7 +755,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="31"/>
       <c r="C7" s="31"/>
@@ -766,7 +763,7 @@
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>0</v>
@@ -964,7 +961,7 @@
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
@@ -973,7 +970,7 @@
     </row>
     <row r="37" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
@@ -981,44 +978,44 @@
       <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
-        <v>20</v>
+      <c r="A38" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="B38" s="31"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
     </row>
     <row r="39" spans="1:5" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:5" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="D42" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42" s="24"/>
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="D45" s="24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E45" s="24"/>
     </row>

</xml_diff>